<commit_message>
Get daily reddit data: Tue Oct 29 08:13:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C499"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3372 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1geok4p</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Got this set done just over a week ago and my polish chipped. Why did this happen? Is the tech using bad polish? Never happened before! So upset with this for the money I paid</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw5jq7rl8nxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1geo7qo</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Having fun with press-ons. </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06ihxmnn3nxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1geo47j</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First design set </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geo47j</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1genn62</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Royal Gemstone Nails 💎✨ </t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1genn62</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1genhz5</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>French Manicure… Thoughts?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygnmxiyaumxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1gemr3j</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Opinions on nail shape</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gemr3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1gem9q5</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Is it supposed to be this color? Online the photos are all clear. Have no idea how long I have had this.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xj219rr2gmxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1gel58d</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Still painting my Murder House Nail Set but here is Violet 🥰</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v93jheu4mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1gelx0n</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Loving the carey effect.</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gelx0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1geln9c</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help please </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geln9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1gelc6u</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>First time using Magnetic Gel!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jcxqhyo6mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1gela0g</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>I’ve been playing around with 3D art. But something about it just doesn’t look right?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jff10o36mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1gel9x2</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Set of press ons I’m working on</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jswi3ml26mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1gel8lr</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>First time doing gel x and French tips!!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gel8lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1gektir</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>The Halloween</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ti5jt3hq1mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1gekncv</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Bl00d splatter 🩸</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gekncv</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1gekka9</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cat-eye tortoiseshell </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0qyvmvs7zlxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1gek7ol</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>First time press ons</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hs7atuzvlxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1gejukw</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Light pink &amp; sparkly </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1c91lhoslxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1gej9up</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Oogie boogie meets jack skellington</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gej9up</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1geiy18</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween nails…can you tell I work with kids? </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qogvu4jpklxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1geiq28</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Cherry Mocha nails 🍒☕️💋</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geiq28</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1geiomu</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal? </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7eouexeilxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1geii1w</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink french  </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh8pomhuglxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1geigcg</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t want to gatekeep great products </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geigcg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1gei4q4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampy nails </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la1nibzndlxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1gehwa0</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>My recent set felt too cute to not share!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gehwa0</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1gehvmo</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Nail ideas</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gehvmo/nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1gehnby</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>GND Gel nail polish</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gehnby/gnd_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1gehgfv</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color suggestions for two different events </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gehgfv/color_suggestions_for_two_different_events/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1gehb5c</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Beware of Manucurist</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gehb5c/beware_of_manucurist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1gehb4w</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Nails for hospitality recommendations</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gehb4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1geh1b7</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My fav set of nails, I've ever gotten</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geh1b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1gef1ko</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>I did not remember polish smelling SO strongly.</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gef1ko</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1gegnh9</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Spooky nails 🎃👻</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gegnh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1gegl9l</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would it be weird if I asked my nail tech for the exact same set she has on right now </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gegl9l/would_it_be_weird_if_i_asked_my_nail_tech_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1gegjus</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall manicure! </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gegjus</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1geghmy</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deathly Hallows ⚡️ </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geghmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1geg2p3</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first self-made raptors </t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/luwy6lsvwkxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1gefz6b</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Coquette nail set 🎀 what do you think?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gefz6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1gefuni</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gefuni</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1gefh36</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Nails and baking: hobbies as a Mom</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gefh36</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1geeoy9</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what’s everyone’s opinions on long, unpainted nails? (they’re slightly blue as i’ve been painting) </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/858e6yf6mkxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1geeg6o</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Is this fast growth?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pnakk4fkkxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1gee61v</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>New set 🤗</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gee61v</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1gee4hp</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Weird looking?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i98di7yhkxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1gedp1q</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails_by_nox on instagram </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbaznklpekxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1gecxkj</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boo! Little chrome ghosties </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gecxkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1gecl1p</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>How to start with gel extension?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gecl1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1gebitg</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>2nd DIY Press On Set</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gebitg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1gece08</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>My fresh French</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd1zwmet4kxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1geb3v0</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Peep the Halloween pedi!!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geb3v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1geayv5</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Moody Carnelian nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geayv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1gea47b</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>First time trying a bright red and I love it 💋</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdlkyzm9ojxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ge9yt5</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>I’m running out of glitters to try at my salon 😩</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge9yt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ge9uo9</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My Libra nail art process</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/986z5pccmjxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ge9n59</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for advice on nail care?? </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a0wzn8vkjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ge8rt0</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got a Japanese high wax manicure on Saturday </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctikdakmejxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ge8lji</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Got my nails done in Tokyo, Japan 🥰</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge8lji</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ge8iag</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Witching season  🌙🐈‍⬛🧹</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13cehldrcjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ge7zdd</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I went to a new place closer to home to get my nails done and they left them like this</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge7zdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ge7vt9</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampire nails. </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge7vt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ge78fy</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got some acrylics what do we think? </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwvhmwmg3jxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ge72zd</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Question About Shaping</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ge72zd/question_about_shaping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ge45n3</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Uneven thumb nail</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge45n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ge6zi8</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>New color of the month 😍 What do you think?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1bb78bp1jxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1gdy3a4</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Pretty nails without damaging my natural ones?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gdy3a4/pretty_nails_without_damaging_my_natural_ones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ge08lg</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bloody Nails 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge08lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ge0k2f</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best top coat and nail glue? </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ge0k2f/best_top_coat_and_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ge1i46</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Fall Leaf Inspired</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puu43piwwhxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ge5762</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>When to get Christmas mani?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k08z236zoixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ge6oxl</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Waited all year to do Uzumaki nails for Halloween. </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmsrs9tjzixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ge60ie</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfs4h4ppuixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ge5zrj</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>i wanna start doing gel x nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ge5zrj/i_wanna_start_doing_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ge5wv1</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>FANCY GLOSS - Mistress Of Evil</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5wv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ge5uak</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did i do? </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lacw3rchtixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ge5tqo</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the difference between these three lamps? </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjk7ibtdtixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ge5eyd</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>In appreciation of my nail tech</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5eyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ge4mk5</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Nail extension options?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ge4mk5/nail_extension_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ge4h8g</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Halloween bunnies</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijny3k0tjixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ge4g5g</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Chipping after a day</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjgl4rkljixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ge473n</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>My spooky set this month. Love my nail tech 🖤</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge473n</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ge4286</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>My latest gelx set - findings ways to do the non dominate hand!</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afak55cugixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ge3s3l</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Tried to make them look like amber</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge3s3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ge3he2</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Is my arch too high for this length?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge3he2</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ge3ag4</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>My design for fall</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlhvse9vaixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ge39pa</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Feeling foresty</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge39pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ge2k9k</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Guy that wants to have his nails done</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ge2k9k/guy_that_wants_to_have_his_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ge2jb2</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Festive Nails! Cat eye edition</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9cw1p2a5ixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ge1oq8</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>My partner did my October nails for me, we have fun.</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge1oq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ge1j6m</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Shape</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0wrcu15xhxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ge0lhb</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth update </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fe61knyohxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ge03x9</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>My newest set🫶🏻</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge03x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1gdzngb</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>first time doing nail art in almost a year 🫶</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gdzngb</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1gdz4tj</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coraline </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gpxf6uy9hxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1gdytha</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Finally bought blooming gel</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cpcadm66hxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1gdys9b</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Halloween Nails 🕷🕸</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0z2qdlbt5hxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1gdygwr</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Black and some glitter</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gdygwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1gdy2xo</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>My fave so far</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/moxjb7z1xgxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1gdxzdz</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>No gems this time but a cute flower to give character🌸</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gdxzdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1geo1k0</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>What about polish pens?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geo1k0/what_about_polish_pens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1gemv85</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Smoking after cuticle oil</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gemv85/smoking_after_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1gem9n3</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Favorite polish of all time?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gem9n3/favorite_polish_of_all_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1gelvoe</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>What should I add to my ILNP Black Friday purchase?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gelvoe/what_should_i_add_to_my_ilnp_black_friday_purchase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1gelrsu</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>can doing gelx give me a nail allergy?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gelrsu/can_doing_gelx_give_me_a_nail_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1gekojc</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Blood splatter 🩸</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gekojc</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1gekkxc</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Guys, I'm gutted....</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gekkxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1gekkuj</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Guys, I'm gutted....</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gekkuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1gekgyq</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloween! </t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ava2q0ddylxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1gekdko</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>ILNP Cygnus Loop🧬</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gekdko</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1gek2ej</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>How to get magnetic French tip w regular magnet?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/utdc5s8lulxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1gejg4u</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Relating a lot to posts about buying polishes</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q522gu54plxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1gehsyy</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>fallen under holo taco’s “love spell”</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2he7yuwalxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1gehpzq</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Magnetic wand trick</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3snl2558alxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1geh95x</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Favorite Matte Top Coat?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geh95x/favorite_matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1geh6ds</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Proof you should be magnetizing your top coat </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02a8txis5lxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1geguki</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>👀 And the banner winner is...</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geguki/and_the_banner_winner_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1gegm6e</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Recs for a 1-3 coat &amp; done deep sapphire that matches my ring</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcrwh5f81lxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1gegehp</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi- raisin’ the bar </t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gegehp</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1gegb2u</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>New-ish to nails. Feedback welcome.</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gegb2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1gefsac</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Galaxy vibes manicure 🌌</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gefsac</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1geegui</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>I free-handed some art! It was really hard, and I’m so proud of them 😅</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wgxj3yjkkxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1geed4x</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beetlejuice inspired nails! 🟪💟🟪 </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geed4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1gedvmh</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you guess? </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gedvmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1gedluf</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Spooky ILNP Gradient</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gedluf</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1gedenc</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>My attempt at a fake blood splatter Halloween Mani 🎃🩸</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gedenc</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ged63z</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Very impressed with Clionadh</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ged63z/very_impressed_with_clionadh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1gecsow</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>What might cause this?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gecsow</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1gec926</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Solution against staining?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gec926/solution_against_staining/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1geby5l</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Your favourite nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geby5l/your_favourite_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1gebv0d</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Mix!! </t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gebv0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1gebrfc</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Halloween attempt</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gebrfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1gebpwh</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Laziness is the mother of invention</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gebpwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1gebacy</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone tried this brand? </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5dwcczuwjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1geb2gg</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Halloween mani 🎃👻🎃</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxzqprt8vjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1geakff</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>LynB Feral Gremlin</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geakff</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1geaja5</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>[TW: Fake blood] First time doing a design</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us5tubbbrjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1geaipj</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October nails </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geaipj</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1gea7ct</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Playing with Sapphire</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gea7ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1gea07f</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>picture polish - cosmos</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gea07f</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ge9t81</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SpOoOoOky cat (or bat)? claws for Halloween week! </t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u198y8c3mjxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ge9lbn</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>The shift is unreal! (LynB Designs - I Did a Punch!)</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge9lbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ge8yy7</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>A subtle Halloween mani 👻</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge8yy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ge8xjt</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>I have a problem 🫣</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge8xjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ge864m</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Day 7 of my manicure</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3vyume9ajxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ge85ho</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>🌕Spooky Night Sky🌕</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge85ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ge79cl</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Cinderella Sparkle</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uenjh87n3jxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ge6kay</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these subtle flakies, part 2 </t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge6kay</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ge6htz</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Homemade dark green jelly using alcohol inks</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge6htz</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ge5zu1</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Base coat for helping to smooth nails?</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ge5zu1/base_coat_for_helping_to_smooth_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ge5xc3</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>FANCY GLOSS - Mistress Of Evil</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5xc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ge5x2r</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Nails for the eras tour</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5x2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ge5x0w</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Halloween mani</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1nqvmettixd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ge5u5g</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Bee’s Knees - It’s Only Magic💚🪄</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7rkclggtixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1ge5pgc</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>this polish has lasted three weeks and still getting compliments 🥰</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5pgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1ge5b5f</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cross My Heart ⚔️ ♥️ </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge5b5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1ge58ra</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Is there anything other than non-acetone polish remover I can use to take regular polish off acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ge58ra/is_there_anything_other_than_nonacetone_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1ge4uwj</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Iridescent white is still a fall color, right? </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/njtq64bjmixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1ge3p45</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>how to keep nail routine relatively stress/mess-free?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ge3p45/how_to_keep_nail_routine_relatively_stressmessfree/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ge3nxe</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polishes like Maelstrom but different colors? </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avo6kylvdixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ge3cq3</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>slytherin. 🐍 autumn vibes. 🍁✨</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge3cq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ge31e2</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>12 days of rose quartz &amp; serenity nails 🩵🩷</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge31e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ge2xsg</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My halloween mani! 🐈‍⬛ </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab9nm5ra8ixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ge2lc4</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Floral Ghosties</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge2lc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ge1s1v</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle Halloween vibes from this polish </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge1s1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ge1jh5</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Help! Ruined my gorgeous pregnancy nails with a bad soak-off</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ge1jh5/help_ruined_my_gorgeous_pregnancy_nails_with_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ge1iu8</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Orly Persistent Memory</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge1iu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ge1e5f</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Matched my nails to my wedding dress 💚💙</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge1e5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ge1977</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chocolate brown for autumn </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0euztcm0vhxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ge0mdj</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Last manicure was over 3 (!) weeks ago - before/after</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge0mdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ge07fv</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Getting into spooky season</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge07fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1gdz6iw</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Concerned Halloween Ghosties</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gdz6iw</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1gdc776</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Help: replacing Cracked Polish brushes</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gdc776/help_replacing_cracked_polish_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1gdj1bn</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scary face skittle? </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gdj1bn</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1gdl3jx</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Color Club</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gdl3jx/color_club/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1gdlcet</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Why won’t my press on stay on?!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gdlcet/why_wont_my_press_on_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1gdnau0</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>preferred base coats?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gdnau0/preferred_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1gdru7v</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Natural Nails Care</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub2o6yqjrexd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1gdycn6</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gdycn6/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1gepbck</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Nezuko inspired nails. By my nail tech at "Oh Fleurs" London, Islington. I love them so much and think she did a great job 🩸❣️</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gepbck/nezuko_inspired_nails_by_my_nail_tech_at_oh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1geos9y</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I did mine and my sister’s nails. What do you guys think?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geos9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1gen0m2</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Hold on to your dookie 👻 💅</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myips3lgomxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1gel507</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Still painting my Murder House Nail Set but here is Violet 🥰</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/112cu51s4mxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1gejst3</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My student designed my Halloween set!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gejst3</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1geiaen</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Spookies nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm14i141flxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1gehy6x</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Candycorn, they could never make me hate you</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf9257n4clxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1gefe0z</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Nail Art Brushes</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gefe0z/nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1gecuzi</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Snowmen live dangerously 😂 I hope I can do the same thing again on my nails.</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6i73xpf7kxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1geclsl</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>More of my Beetlejuice nails 🪲</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geclsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1geb1w3</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>hey I'm back👻</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geb1w3</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1ge9vuz</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Hallowen season 👹</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19t0q9nmmjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1ge9u1c</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Some bones</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge9u1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1ge8llb</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>I did my nails for Halloween:)</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7evafifdjxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1ge4jol</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My design for fall </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27eynbl3kixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1ge47ik</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Halloween designs 💕</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge47ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1ge40fz</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Asking tips for applying metallic/glitter powders</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ge40fz/asking_tips_for_applying_metallicglitter_powders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1ge3zmj</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Got a chance at a redo, I’m so proud &lt;3</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dnq02zagixd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1ge3g0v</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Hand painted ghosties that glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ge3g0v</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Oct 30 08:11:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C499"/>
+  <dimension ref="A1:C695"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8916,6 +8916,3338 @@
         </is>
       </c>
     </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1gfhc5v</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>October nails!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfhc5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1gfh00q</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did nails by myself and took those pics in my parking lot for more holographic effect! </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfh00q</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1gfgvkg</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Green Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfgvkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1gfgipc</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>How can I stop the split?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfgipc</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1gfgg2a</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Halloween Glitter Gradient 🧡🖤</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfgg2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1gfgd2c</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Late to the spooky nail club</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f84kxs14auxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1gfg81p</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>What nail shape would suite me best?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07ket1u78uxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1gffz09</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">trying subtle spooky designs </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/galt0fwt4uxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1gffnmz</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Salon doesn’t need to prep it seems!</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gffnmz/salon_doesnt_need_to_prep_it_seems/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1gfflpy</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Any brand recommendations that make small press ons?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfflpy/any_brand_recommendations_that_make_small_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1gffcyv</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>⚠️Trigger warning ⚠️ flashing and strobing gif</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvg7c2ixwtxd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1gff3o5</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Gel Nails Popping Off</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gff3o5/gel_nails_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1gfeanc</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail dilemma!! </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfeanc/nail_dilemma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1gfdxhh</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>can always rely on press on nails for a last minute manicure 💅🏼</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1tjx99lgtxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1gfdsg8</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Pochacco Nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfdsg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1gfdikt</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween press-ons, and the set I did for my niece </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfdikt</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1gfczc7</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>press on nails</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfczc7/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1gfcmy2</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally grew out my natural nails after being a nail biter for 25 years! </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/po2zwcsp3txd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1gfc4wp</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>matte black &amp; chrome ♡ *:･ﾟ✧*:･ﾟ</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57zl6z11zsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1gfc09d</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>red &amp; gold nails !</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfc09d</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1gfbxyy</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Apres XL Square! 🤩 </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfbxyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1gfbwcn</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stilettos in the office. </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n92q0ylpwsxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1gfbon6</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 👻🎃</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baqn9jcxusxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1gfbee7</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>My Halloween set 🎃 I love my little friends 🥹</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlzggjbcssxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1gfb4jf</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Where to buy good quality efile bits</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfb4jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1gfamco</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A *huge* thank you to everyone here who has recommended a glass nail file!! </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmk6pgcdlsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1gfaisi</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting my nails done! </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1znds3iksxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1gf9fb8</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Best press on?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gf9fb8/best_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1gfa057</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Minimal Style, Halloween Vibe</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upuc2fq2gsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1gfa7z9</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Candy corn! 🎃</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y53zo8xxhsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1gfa5xh</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>I did the vampire fangs thing</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n35d67cghsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1gf9plf</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>New set ✨️</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czsxg08kdsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1gf9b0r</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Girly Halloween 👻🩷</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf9b0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1gf97of</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>need fall colors for my nails</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gf97of/need_fall_colors_for_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1gf89q6</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails match my favorite drink! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va6pnyzl1sxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1gf83ow</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t01uwoqa0sxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1gf82bf</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My natural nails! </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpcl30yzzrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1gf7yjb</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Zebra print BIAB nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc7hdzg3zrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1gf7bqe</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Made for the prettiest bonita🥰</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fi5apu2xtrxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1gf6mov</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">please please help </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gf6mov/please_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1gf6iap</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Suggestions for shape/length?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w68697wgnrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1gf5qxq</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>How obvious is it that these are press ons?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf5qxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1gf4wrk</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>something simple - pinterest inspired 🥀</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwoydjpebrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1gf4kx8</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf4kx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1gf4cv2</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf4cv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1gf3qha</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Polish won't stick</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf3qha</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1gf3tf3</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Desperately looking for this nail polish!!</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y4wjdda3rxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1gf3o83</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest opinion on my Biab manicure? </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/937j8ch52rxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1gf3dw6</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Gel match for ILNP Chleo</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy96uynzzqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1gf2vuz</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Tips for Gel</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf2vuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1gf2qgn</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Tried gel nail paint for the first time! A lil Halloween  design :)</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf2qgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1gf22tl</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Conni Reinforce Gel Uses?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4umylrfqqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1gf2dsy</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>been a nail biter my whole life, using builder gel and this is a month of growth!!!!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf2dsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1gf2a0y</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Vamping it up with these Blooodddyyy nails</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzqjjr0xrqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1gf25td</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>do press-ons belong here?! so happy with this set 👻🦇🖤</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0iv27d1rqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1gf25rn</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Alexa, play Another Life by PinkPantheress</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf25rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1gf21xk</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Husband called them Thanos stones 💎</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf21xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1gf1zzx</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gothic cross nails for the spooky season </t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf1zzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1gf1por</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Simple little Halloween design🦇🦇</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsh9ypxqnqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1gf1kgc</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>What do you think of this owner who did it yesterday for a wedding?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiwv3moomqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1gf1gw3</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Nails for the week 💅🏾✨</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcx04fcylqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1gf1cyq</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxcqbqr5lqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1gf0zpx</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Extending side of nail with acrylic?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bocdc5khiqxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1gf0rhb</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>3rd week of spooky season</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf0rhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1gf0oo1</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>What to use to attach gel x</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gf0oo1/what_to_use_to_attach_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1gezmf8</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>How do I ask for something more natural looking for nail extensions?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gezmf8/how_do_i_ask_for_something_more_natural_looking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1gezve1</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Help with health of nail.</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gezve1/help_with_health_of_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1gezwm9</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Your thoughts?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gezwm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1gezbk8</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Question about nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gezbk8/question_about_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1geyzca</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Advice on what to do with my nails?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geyzca</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1geyet2</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t xml:space="preserve">6 hours later </t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geyet2</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1geye1k</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>I love my nails because they kind of look like amber?🤎🩵</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7kodkg9zpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1get676</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Just unknowingly got a Russian manicirw and fainted during the procedure</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1get676/just_unknowingly_got_a_russian_manicirw_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1gevhfj</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Ideas please! (Fairy)</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2dhd3h6dpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1gey142</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>New to nails. Does this shape look ok on me? Second time getting them done but still don’t know what to ask for.</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpv9xn6pwpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1gexzc0</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloween </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qybq77jbwpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1gexvrd</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>▫️</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysjlj6alvpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1gextq6</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Bi pride nails 💗💜💙</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gextq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1gexjh0</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>I have never had nails long enough for French tips before but finally managed to stop biting and get my dream manicure 🥰</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gexjh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1gexhqz</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Slim French tip on my natural nails. First time getting my nails done in 2 years!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gexhqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1gexdp9</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Does anybody else use a gel topcoat to make their lacquer-mani last longer?🌹🥀</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gexdp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1gex189</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>What color is this?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud5wn5n6ppxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1gex0gp</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Nails tips?</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxal9do0ppxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1gewwdv</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>I’m obsessed with my new nails🩷 completely hand painted 🥰 what do you think?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9sqcka5opxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1gewmps</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Gold chrome tips for the win🤌🏻</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wraltym4mpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1gewlom</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>🎃My Budget DIY Halloween Nails!🎃</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jpypu9wlpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1gewk0k</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Do this shape and lenght look good on me?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gewk0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1gew8h3</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Nail shape/design advice?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gew8h3</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1gevw0f</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Spooky Ghosties 👻</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/489cf4hagpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1gevr8u</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>First time posting here🍷♥️</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17kchy38fpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1gevljv</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>What’s your favorite vampire movie?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuii4im2epxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1gevbie</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing Gel X on myself </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwme5xxxbpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1geujs4</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>What do you think</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5jrfshj5pxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1geu07h</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Cat doesn't like my poorly attached Halloween pressons</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geu07h</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1getw9g</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>🩷🩶</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1getw9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1getbe7</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape fits my hand? </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7ak7vfxuoxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1get2p6</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>My last few sets of Halloween nails. Pretty new to press ons. Any tips?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1get2p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1geshox</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Short and naturals nail... give them rest from polish and gel\acrylium</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jbudsx7moxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ger2e9</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>We love a basic 🍒</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9x0ka9z6oxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1geqll4</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting nails done </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vf5wevy0oxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1gfhghr</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's the strongest velvet magnet available? </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfhghr/whats_the_strongest_velvet_magnet_available/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1gfgyv7</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Can’t stop looking at my nails 🍁</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahfbyb6qiuxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1gfgft7</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Halloween Glitter Gradient 👻</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfgft7</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1gfg5x7</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>in search of a brown crème polish with slight shimmer</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4391gve7uxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1gffjda</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Tried a new thing 🙂</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/29-10-2024-6KnqXCJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1gff35t</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just in time for Halloween! </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo5d2s8ittxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1gfezaa</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>What polish comes to mind when you think "bright red"?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfezaa/what_polish_comes_to_mind_when_you_think_bright/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1gfetyq</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Looking for a nail polish like these press-ons?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfetyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1gfesre</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dream within a dream </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfesre</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1gfeg7e</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>a Goblins and Ghoulies appreciation post</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/au2nb7q5mtxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1gfc58o</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Black Linear Holo Recs?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfc58o/black_linear_holo_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1gfbx0s</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Dupe for Chemistry</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfm92ny0xsxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1gfbrcf</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Catrice </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfbrcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1gfbqcr</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Mana with Pulp 🪄💙</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/id5gtv00vsxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1gfaq6t</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Loving this LynB</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dfr0k1z9msxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1gfa3ql</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>I don't think reflective glitter is for me</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfa3ql</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1gfa1r4</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this color so much I can’t stop buying more shades … </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfa1r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1gf9plx</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t xml:space="preserve">oliveandjuneus.com a scam? </t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf9plx/oliveandjuneuscom_a_scam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1gf9mc6</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>I’m hooked!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf9mc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1gf9m1c</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>OPI Black Spotted not spotting. Can I save it?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf9m1c/opi_black_spotted_not_spotting_can_i_save_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1gf8w34</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Super happy to have snagged Coronation this time around!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwuv4knm6sxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1gf8imn</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Birthday Brat 🩷😝</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf8imn</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1gf86kv</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Flowerchild + MyMelody</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf86kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1gf86av</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Wicked-themed Skittle</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf86av</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1gf81u2</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art for Halloween!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1oh6pamvzrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1gf7mmj</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Low energy Halloween nails</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf7mmj</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1gf7a1v</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my algae + glitter nails (ILNP Countryside) 🦠 💖 </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf7a1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1gefbzr</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Nail Art Brushes</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gefbzr/nail_art_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1gf71ah</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Halloween nails + dog tax</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf71ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1gf6wfc</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Anyone looking for Smith &amp; Cult? I have about eight bottles in different colors... Most unused and unopened.</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf6wfc/anyone_looking_for_smith_cult_i_have_about_eight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1gf6qrc</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Suggestions for a deep teal polish</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf6qrc/suggestions_for_a_deep_teal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1gf6mqj</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>ILNP - Eclipse 🌘</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf6mqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1gf6me1</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>The only thing in my garden the groundhogs didn’t eat was this dead gourd. (Cirque Eye of the Beholder.)</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cp4zegldorxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1gf6iuk</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>My favorite polish!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf6iuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1gf6fc5</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Happy halloween!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf6fc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1gf5qoo</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>lynb designs ATE</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf5qoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1gf5qlr</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Anything similar to this Chanel polish I keep ogling at Sephora?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf5qlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1gf5pa3</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Regular polish that looks like this?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jslim6k8hrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1gf5ld1</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Tried to recreate the Galaxy vibes</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/87mobx9egrxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1gf5klg</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>🧪🎃👻🔮</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qeifzxs9grxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1gf5gwv</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI My voice is a little Norse </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i74ppijkfrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1gf5fo8</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Magnetic regular polish help!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf5fo8/magnetic_regular_polish_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1gf57cg</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>run don’t walk to your nearest Marshall’s 🏃‍♀️💨</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ir4ulrkdrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1gf491z</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Sunset in a bottle</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf491z/sunset_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1gf48nn</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m jealous of all of you with perfect manicures. This is hard! </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf48nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1gf419b</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>All my colour nail polishes!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ely4vzru4rxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1gf3su0</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Desperately looking for this nail polish!!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p1gavz53rxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1gf3dbx</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>A Glow Up</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf3dbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1gf35sa</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>How long do you hold onto a polish you hate before tossing 🤨</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf35sa/how_long_do_you_hold_onto_a_polish_you_hate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1gf2jgu</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>ILNP Lily 💜</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w27byhvtqxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1gf1zxo</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bloodborne inspired mani in the spirit of Halloween </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf1zxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1gf1kj2</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Polished for Days Quite Literally Dead Inside</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf1kj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1gf1kdz</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>I never should have joined this blasted subreddit! (Collecting since 08/24)</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf1kdz</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1gf1din</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Today's polish! Sassy Sauce &amp;Mooncat</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf1din</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1gf0r1x</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Couldn't decide what to do for Halloween so I did it all. My spooky night sky maximalist Halloween mani</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf0r1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1gf0l9t</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not getting any work done </t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r16npn9jfqxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1gf0leg</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Beaux Rêves - Blooming Azalea 😍</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu8wr0zjfqxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1gf0ho4</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Tigers eye polish</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gf0ho4/tigers_eye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1gezpyx</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Glow in the Dark Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gezpyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1geznmg</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Jazzed up candy corn mani (plus bonus spooky season colors)!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1geznmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1gezay2</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Paranormal Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gezay2</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1geyd0h</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Please recommend label makers for swatch sticks!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geyd0h/please_recommend_label_makers_for_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1gexrif</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Does anyone know when OPI Infinite Shine Stay &amp; Night was released? Looks like a dupe for Julien's Greyt but I can't really find anything about it</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gexrif/does_anyone_know_when_opi_infinite_shine_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1gexcfx</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Nail shape advice</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gexcfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1gewtik</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>So, um... Is it normal to have a pile of polish that disappoint in this hobby? Can't help but feel I might be doing this wrong haha</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gewtik/so_um_is_it_normal_to_have_a_pile_of_polish_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1gewqo1</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Brand New</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gewqo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1gewiwv</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>My first great experience with magnetic polish 🌌</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gf8004ualpxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1geufsj</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Today's mood: ⛈️</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpu662mo4pxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1getp4q</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>sp00ky mani 👻🕸️🦇</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1getp4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1getiq0</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Spiderwebs</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1getiq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ges2v1</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail/Skin Biting &amp; Picking </t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ges2v1/nailskin_biting_picking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1gerncc</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Does this shade of nude polish look OK with my skin tone?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gerncc</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1geqpbp</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Your holy grail AM + PM hand cream?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1geqpbp/your_holy_grail_am_pm_hand_cream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1geq1u7</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>This holographic silver 😩💖</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z59i26xhtnxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1gfgeg1</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Just did my own Halloween nails!!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfgeg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1gfg5v5</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I love these 🥰</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfg5v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1gffs8c</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my first nails </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6r03ui2d2uxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1gfehvp</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First five of my first Christmas set! </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef793llomtxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1gfe6t8</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my nails </t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voarqggdjtxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1gfcd2o</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I enjoyed tris set </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfcd2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1gfb58c</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Issue using Q-tip for design</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gfb58c/issue_using_qtip_for_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1gf7pbf</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Do you like it in black and white?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u05qrvzwrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1gf6grw</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween French tips </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf1gtxi4nrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1gf678r</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Not the greatest artwork but here are my Women’s Rights nails!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzg7n893lrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1gf4xq8</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boo👻👻 </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et0mx2xlbrxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1gf4x4n</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got them done for Halloween! </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf4x4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1get6s5</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>First time nail art</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5m8n0gotoxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1gexwf4</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Spidey Senses. Working on glazed nails with regular polish</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47snxz3qvpxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1gf0pyc</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd week of spooky season </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf0pyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1gf0f28</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Check out my new ghostface nails did them myself all hand-painted 😊❤️💅</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gf0f28</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1gf009v</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>My little sister is studying, these are the first things she has done for me. what do you think?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv2elo18bqxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1gewdn6</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spider nails </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gewdn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1gewblw</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Halloween Art contest</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gewblw</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1gevmpl</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>What’s your favorite vampire movie?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36c3usacepxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1gefmey</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Haven't posted in years, but here's a recent set I did 😍</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74qcrm70tkxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1gepo6i</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>cute i love it</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tesiffj1onxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Oct 31 08:10:55 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C695"/>
+  <dimension ref="A1:C882"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12248,6 +12248,3185 @@
         </is>
       </c>
     </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1gg975p</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>top coat dulls sparkle</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg975p/top_coat_dulls_sparkle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1gg8p8r</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HAPPY HALLOWEEN 🎃 🤪 </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg8p8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1gg8gyg</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Gel polish or regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg8gyg/gel_polish_or_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1gg8953</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Pressons ready for Christmas</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg8953</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1gg7ptv</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>been using press-on nails for 4 years now, here are some of my favorites</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg7ptv</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1gg6u18</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>What is this clear stuff under my nails?</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5go5s9h8w0yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1gg73bo</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Do I need a new set?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/liy33yj4z0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1gg6z7u</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amv3pzxwx0yd1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1gg6i26</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>My fall nails ✨</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6i26</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1gg6hy0</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>First time i did colored french nails, still getting used to the look of them 💅🏻</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6hy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1gg6ek4</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I avoid this </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6ek4</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1gg6bhq</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Manicures don’t last at all</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg6bhq/manicures_dont_last_at_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1gg61yu</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Fresh color</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg61yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1gg5zyg</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Favorite Set I’ve Ever Gotten! </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mmgnh91n0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1gg5syi</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Not in season 🌸</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azxacug4l0yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1gg5rrr</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg5rrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1gg5kbq</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wedding nails (not my wedding) </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0c0ct0xoi0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1gg56ni</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Silver Celestial Nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ern29wxse0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1gg562w</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>First time doing nail art (student)</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v49b1k3se0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1gg4zkx</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Sister in law Joked that I have “Wrinkly Old Lady Hands”, now I’m Self Conscious. Any Hand/Nail Care Product Recs?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzvro5dzc0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1gg4da8</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My spooky nails inspired by my boo wala 🤭</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00tu13a170yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1gg4jh2</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Outlast Video Game nails just in time for spooky season!!!! 🫣</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhu67o3o80yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1gg4i7o</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Opinions? 😊</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg4i7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1gg4do6</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Language barrier/terminology </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg4do6/language_barrierterminology/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1gg3r5t</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>First time getting polygel</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg3r5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1gg3kyv</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first splatter nails to match my halloween costume </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jezeonwzzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1gg37un</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>She's an Oklahoma smokeshow 🎶</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qvuo2bkwzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1gg36op</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is there any advantage to Dip or Gels ? </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg36op/is_there_any_advantage_to_dip_or_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1gg362l</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>First time fall nails by me</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg362l</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1gg2zit</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Never had my nails done, what colour would suit my skin tone? </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnhcp1hjuzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1gg2t1f</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Going for gold and black Halloween vibe 🏴‍☠️🎃</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fko5xtd0tzxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1gg2k7a</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Playing with cat eyes gels</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/10qxk8jrqzxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1gg2hfl</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Halloween set I did myself this year!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg2hfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1gg2eb0</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Hey everyone need some advice!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg2eb0/hey_everyone_need_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1gg26nc</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Gel Polish Question</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gg26nc/gel_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1gg1wg0</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>sometimes less is more ✨</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut3xyth7lzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1gg1lpq</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>What I have now and going for my fill Saturday!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dob667epizxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1gg098j</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Am I overreacting? I went to get my gel polish taken off so I can give my nails a small break. This is the state the nail lady left my nails in… I would of just picked it off had I would of known she would damage them this much 😭</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x003ducr7zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1gg19li</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>🖤 it's basic, but I like it</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8pxqepxfzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1gg0voe</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Custom Harley Quinn set 🃏💋</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/719fqmkqczxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1gg0l8d</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What can cause this? </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bikldereazxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1gg0hrv</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Waiting for Halloween </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85mg2imn9zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1gg09vi</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Birthday sparkles for me</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s66pxdw7zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1gg084d</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>best acrylic set i’ve ever had</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65fibski7zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1gfzv7d</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>got halloween nails!!</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjizi0hn4zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1gfzc9h</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My nails look appetite 😋</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1i6v7pmg0zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1gfzbpe</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>simple birthday set ✨🦂</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buicr0hc0zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1gfzb80</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Any advice on how to file stubbier natural nails while they're growing out?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfzb80/any_advice_on_how_to_file_stubbier_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1gfz6ib</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Ops... I did it</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfz6ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1gfyhim</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Gels nails lasting</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfyhim/gels_nails_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1gfytff</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Pink and black glitter ombré 🖤💖</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2oszf1bwyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1gfykiz</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Cutie Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfykiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1gfyhsf</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Good or bad? Be honest.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfyhsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1gfxy3i</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a question about powder dip nails </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfxy3i/i_have_a_question_about_powder_dip_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1gfxbe9</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfxbe9</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1gfx968</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>How bad are these??</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfx968</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1gfx4q7</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Care tip: apply vaseline to nails after removing old mani</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfx4q7/care_tip_apply_vaseline_to_nails_after_removing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1gfx1i0</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>First attempt at isolated chrome, nubbies again.</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/is6z3dboiyxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1gfwycq</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>doodle nails 🌀*️⃣🛁</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twn8y6q1iyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1gfwwko</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>I got the cutest little ghosts for Halloween!! ❤️👻</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kltzofknhyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1gfwmxx</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Off season but On point for beach vacay ^_^</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfwmxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1gfwhc3</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape will look good on me? </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfwhc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1gfwcn7</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Into keeping it simple lately</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd2ywulbdyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1gfvls0</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Gel polish doesn’t cure around cuticle?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfvls0/gel_polish_doesnt_cure_around_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1gfvwnq</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on this nail colour </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i8kmcl2ayxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1gfvuiu</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Halloween Set 👻🕷️🍫</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfvuiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1gfvrd1</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Filing Gel Off- Nails Now Super Weak!</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfvrd1/filing_gel_off_nails_now_super_weak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1gfvqz1</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Colourful Swirly Whirly Nails by me!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfvqz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1gfvj4a</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Witch season 🎃</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sq7x3n97yxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1gfvgma</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm very proud of these!!! </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brurhv1q6yxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1gfvbbn</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Third Halloween set (DIY)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfvbbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1gfv9ok</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Demon Slayer INDEED</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ggd97i695yxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1gfv0hq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I just keep painting over old gel polish with more gel polish? </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfv0hq/can_i_just_keep_painting_over_old_gel_polish_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1gfusn7</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>obsessed 🤩😂💋💘</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfusn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1gfukou</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Dip products</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfukou/dip_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1gfud5r</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Halloween set</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfud5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1gfu7k1</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Spooky Nails Vibe 👻🧡</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfu7k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1gft3la</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying press ons! </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74xfqwe0pxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1gftexo</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>So sparklyyy ✨</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmq1ix6drxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1gfsyux</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which nail shape you think will suits my hands ?  </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w7z5kd1oxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1gfsn35</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>My Halloween nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfsn35</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1gfseis</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>A set that took me hours to make this week.</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6oly2vxjxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1gfsd3a</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Chrome nails chips easily?!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy0z5ynmjxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1gfsbn7</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Help I need advice</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfsbn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1gfrebw</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>a lot of doubts about nails</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfrebw</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1gfrwfv</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>In love with this colour combo ✨️🍂</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl08uk08gxxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1gfrtu1</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I love this red </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5pcucqofxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1gfrtkl</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd Halloween set </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sv8t0dlfxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1gfrt7v</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time press ons </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii5n975kfxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1gfrh0p</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diy gel over dip experiment </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39nl1f13dxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1gfr1fh</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Halloween nails (natural)</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baauxlit9xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1gfr1xv</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I'm fall...ing in love with this 🤎✨️</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfr1xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1gfpypc</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gfpypc/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1gfqnie</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Halloween but.. neutral?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfqnie</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1gfqgo9</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Can somebody help my nails?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfqgo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1gfq8bj</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐆 🍒 </t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmydqlgr3xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1gfq01h</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2c9vp142xxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1gfpv6c</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Hello Sidney…</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfpv6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1gfh1xe</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Who's jealous of my pedicure?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51485o80kuxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1gfjm8t</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Obsessed with these elf stone opal nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfjm8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1gg8n62</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Delusions of the Eclipse</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/18nfmz9kj1yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1gg6u5t</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>ILNP Truffle &amp; Cirque Velvetine</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6u5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1gg6rqv</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6rqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1gg6qzv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>ILNP Starlight</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6qzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1gg6nh7</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Nails lifting from bed</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iha7f8s5u0yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1gg5utu</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Black with rainbow sparkles for Halloween!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ndd6voiml0yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1gg4jjg</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>slay!!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg4jjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1gg3x15</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Indie Black Friday Sales</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gg3x15/indie_black_friday_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1gg3dnr</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My halloween gradient! </t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtn8ggd1yzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1gg3ajt</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>SCREAM</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg3ajt</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1gg38pd</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPIxWicked Defying Gravity </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg38pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1gg2f8s</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>For Halloween</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9p8068npzxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1gg1uo9</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>For a vacation release it's such a great Halloween color</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhxgmourkzxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1gg18y9</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Stupid question: I bought press ons and there aren’t enough big ones to fit me. What now?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gg18y9/stupid_question_i_bought_press_ons_and_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1gg0dhr</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>First Skittle!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg0dhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1gfzoqq</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Mooncat Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cflbv8p63zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1gfzeo7</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Choose my nail color!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acxvkz5z0zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1gfye60</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>A Halloween Prugly for the Ages!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucvkrk1vsyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1gfy833</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Quick Dry Polish Recommendation</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfy833/quick_dry_polish_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1gfx39u</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some last minute Halloween nail art 🩸 </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfx39u</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1gfwxwp</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>this year's halloween nails! 👻🧡💜💚</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfwxwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1gfwg7l</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>BKL Bad Manners</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyecv3l6eyxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1gfw9on</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>October Mani recap!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfw9on</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1gfw3yk</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Halloween nails! 👻🎃</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfw3yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1gfvmd8</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Thermal Ghosties!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfvmd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1gfvckb</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Cirque Fools Paradise is 🤌🏽</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f6ff404u5yxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1gfv6xv</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Sexy Demon Slayer INDEED</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hjbrusln4yxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1gfv29n</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Fall Fave: Mooncat in “Pomegranate Seeds”</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfv29n</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1gfuy8p</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Witch House for the week of Halloween!</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f2s5p91r2yxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1gfu7qz</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Halloween ish</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcqfh4p9xxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1gftv3l</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Just got my order from LynB</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gftv3l/just_got_my_order_from_lynb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1gftp3o</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy with my first Halloween claws in a long time </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gftp3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1gftkrr</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Yellow Calaveras</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gftkrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1gftg9n</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I swear they’re all different </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lakbb18nrxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1gfshz5</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For Peter - Phoenix </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfshz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1gfsgba</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Gave magnetic gradients a try 🧡❤️💜</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8gb5tldvjxxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1gfrxow</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for hg utensils or products for at home manicure </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfrxow/looking_for_hg_utensils_or_products_for_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1gfrsz9</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Halloween velvet</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cmh9ik6gfxxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1gfrqsv</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Bee’s Knees It’s Showtime!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfrqsv</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1gfrh47</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child over Essie In Plane View</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfrh47/ilnp_flower_child_over_essie_in_plane_view/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1gfr4vk</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Favourite Colour Pallete</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfr4vk</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1gfqz72</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr5qvp2d9xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1gfqxkr</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>🕸️Spiderweb nails 🕸️</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfqxkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1gfqqpc</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Fool's Paradise</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfqqpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1gfqq6y</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>this color is giving me ”vogue trash bags”</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12u45uih7xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1gfqmbv</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>What’s the difference between a “quick dry” polish and a normal polish ingredients-wise? Just curious</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfqmbv/whats_the_difference_between_a_quick_dry_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1gfqa9h</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Stash </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dv01zuh54xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1gfq4nj</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Nail snape - keep or go almond/oval</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tq18ao03xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1gfq3q2</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My favorite Halloween polish 🎃</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kvvzilt2xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1gfpufk</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Home made press on nails </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfpufk</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1gfoxzh</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Halloween, but make it sparkly</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm705t64uwxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1gfoqck</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>How to use ring magnet?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/viwh61mjswxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1gfopkq</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Icebreaker by Polished for Days</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2nmitkhdswxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1gfomaf</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>🍎💚Poison Apple💚🍎</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfomaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1gfojx9</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Simple look for Halloween</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5e25exbrwxd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1gfo8p2</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzdjn8uuowxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1gfmecp</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Feuillemort!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfmecp</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1gfm53w</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Has anyone used Duri?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqoggbqv7wxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1gflmv8</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">so proud of my lil ghosties 👻 </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gflmv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1gflmo2</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First almond nails! </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gflmo2</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1gflimq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>I have no words...</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uzrzth872wxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1gfl8dh</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Tfw you finish your mani and... you don't like it one bit 😡</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xopu5zrlzvxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1gfkkkc</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pumpkins!! 🎃 </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfkkkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1gfjkul</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sorry in advance for this absolutely dumb question </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gfjkul/sorry_in_advance_for_this_absolutely_dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1gfitnr</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloween! 👻💜⚓️🖤🧟‍♀️ </t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfitnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1gficat</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>I just want a plain coating on my nails. Would just a base coat + top coat work? (Without any other polish)</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gficat/i_just_want_a_plain_coating_on_my_nails_would/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1gg7skp</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>First try to paint my own press ons. How did I do? Any tips?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg7skp</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1gg7oc2</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>halloween set</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg7oc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1gg7bnx</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>10 hours of work later..</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg7bnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1gg6j1g</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Halloween Set</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg6j1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1gg56jd</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>First time doing nail art (student)</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgx0wykwe0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1gg547i</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>thought i’d share the set i made to wear for halloween tomorrow! 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm9dpx5ae0yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1gg48xy</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galáctico </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8o527fz50yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1gg1xau</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>1 or 2?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg1xau</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1gg0hwy</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>With this set, I finished my long day of work.</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azjn9e1p9zxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1gfvd9q</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry Nails 🍒 </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nx2dray5yxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1gfvcm6</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>I tried embossing with gel and encapsulation</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y97q0cvq5yxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1gfv64k</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Third Halloween set</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfv64k</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1gfuk9c</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>My Halloween Set, Recs on Good Detail Liner Brushes?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjrisyrpzxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1gfswvi</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfswvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1gfshlo</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I made this design yesterday, I really liked them.</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvt8zhvjkxxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1gfrkv0</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Melon Soda Nails!!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfrkv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1gfq9j7</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today i said that i’ll do a soft design, something quick but i never keep my words haha </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ly4my6804xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1gfpzd0</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Please don’t kill me Mr. Ghostface! I wanna be in the sequel!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfpzd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1gfprxw</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>another halloween pink</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv2oyfwc0xxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1gfmqjq</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Set! </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrrjtn0wcwxd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1gfjr0u</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Spooky nails for Halloween</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfjr0u</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov  1 08:11:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C882"/>
+  <dimension ref="A1:C1088"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15427,6 +15427,3508 @@
         </is>
       </c>
     </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1gh0aij</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Tried mismatched gel nails for the first time 💜</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh0aij</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1ggz2jo</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Found These Mini Scented Polishs The Other Day</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggz2jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1ggysdn</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>My botched gel manicure 😢</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggysdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1ggyiqb</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Diwali nails </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4e7hsm8l88yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ggy2u7</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Halloween hangnails 👻</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feelgaq138yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ggxks4</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>When red becomes a personality trait 🍷</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggxks4</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ggxerq</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Halloween set!</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p24xcsi6v7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ggxczk</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Happy Halloween! Pink cat eye with spider webs… painting thin lines on my opposite hand put a whole new meaning to anxiety 😅</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vadlu1xdu7yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ggwe69</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>This years halloween set 🕸</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m4h3eedk7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ggvk5b</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Meow </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crct3rhqb7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ggv5ev</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggv5ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1gguvwb</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Love these 🥰</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3o9cwe057yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1gguvtr</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some cute Amazon stickers and a sleepy girl </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi920krz47yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ggugzt</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Halloween nails to match my ring 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggugzt</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ggug4d</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>love this set, both hands are different</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggug4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ggt8m0</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November nails tiiime! </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ti453kbgp6yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ggt6n4</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Look at that glitter blue color, is my favorite by far </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/que93dwxo6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ggsyl6</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bog15mpwm6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ggr9tc</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>My first time!!</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggr9tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1ggr6qn</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>This is NOT what I asked for…it’s everything and more 😍</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggr6qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1ggrmsh</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need advice please on what I should do </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggrmsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1ggs0dw</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Did these nails, not halloween but I love</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bujz1u7ie6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1ggs4iw</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Short but cute</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/23n1zt4jf6yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1ggs4cy</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went for a basic V french this time </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/355tokzhf6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1ggrur4</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🖤 chrome </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hb66zsu3d6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1ggr8db</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for someone who knows nothing about nails </t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggr8db/advice_for_someone_who_knows_nothing_about_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1ggqtky</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>My Halloween nails 🎃</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8njjjyz36yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1ggr27s</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Tips on practicing gel art on yourself</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggr27s/tips_on_practicing_gel_art_on_yourself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ggqwg3</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>what color should i try next?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c11x3xnp46yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ggqlfq</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>5 days growth</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vxoyw7326yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1ggqc0x</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Witchy vibes and my kitty helper 🐱 </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggqc0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1ggq72h</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Dupes for this nail color?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rogvs6qy5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ggq6mp</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Día de los Muertos </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggq6mp</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1ggq699</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Back to my roots after a looong nude phase 🖤</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggq699</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1ggpylg</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Bare acrylics</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggpylg/bare_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1ggptnj</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Is my apex in the right area? (beginner)</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggptnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1ggpubb</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Did my nails for november</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggpubb</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1ggphuk</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prepping for December </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eu1fyt9zs5yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ggny3i</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So Jack was my inspiration </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p33zc08ng5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ggo8sr</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>What kind of nails would work well for me?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkbvx380j5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ggolml</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>yall help me pleaseeee</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggolml</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ggp778</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple Vibes </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55llqd1mq5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1ggom54</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>My first magnetic mani 🤍🩷🤍🩷🤍</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dks3in6yl5yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ggof31</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>nails for today :-)</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa4uqz8fk5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1ggof3b</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Spoopy lil ghosts</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggof3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ggoen9</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail tech </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dydjjtmak5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ggobtb</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to show off my nails ☺️💜 </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggobtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ggnk0o</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Glue/Sticky Tabs removal</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggnk0o/gluesticky_tabs_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ggnu4i</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Those Kiss Impress peel and sticks….</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggnu4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ggn7ep</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Did my first press on nails in the car while being a passenger princess haha</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggn7ep</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ggn685</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Don’t ever let anyone tell you that women only paint their nails for men</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggn685/dont_ever_let_anyone_tell_you_that_women_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ggmc3u</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cateye is just.... Yes!!! </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf74v7od45yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1ggm0t3</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Removing nail glue</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggm0t3/removing_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1gglzzd</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>made some pressons to match my costume!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd9zc7vu15yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1gglxea</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Halloween/wedding nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzelrb4a15yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1gglg2s</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Builder gel under Gel X ?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gglg2s/builder_gel_under_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1ggktw2</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Tortoise and gold nails! 🐢✨</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udpjc27xs4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1ggl5d1</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Sick and staying home but at least I have my Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggl5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ggkx9i</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloween! Last day with my spooky set </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g95f41wlt4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ggjpuy</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>record breaking no chips after 4 days 🥳🥳</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggjpuy</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ggjgrz</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ℍ𝕒𝕡𝕡𝕪 ℍ𝕒𝕝𝕝𝕠𝕨𝕖𝕖𝕟 </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/loy5ukjdi4yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ggjdc9</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfgw5y2oh4yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ggjd2p</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Halloween bats set</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggjd2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ggj1pr</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Happy Halloween!! 🎃</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggj1pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ggirw5</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic but glitter ✨ </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gd6ta69zc4yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ggikmq</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Another one I did on myself (beginner)</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr07jpshb4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1ggib0v</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this considered squoval? </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isfsneag94yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1gghwdu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Help me understand the services pls?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y6jr2ve64yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1gghuip</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>How did THAT happen?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kjex3b064yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1gghqw8</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second attempt </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gghqw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1gghopv</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gghopv</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1gghl43</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>My rainbow nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gghl43</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1gghkry</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Nail growth help</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gghkry/nail_growth_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1gghjdm</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>This is Halloween 🎃</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j7ktmxl34yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ggh8cx</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>🎃👻</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9zoguq914yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1gga9cv</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How do I fix these nails?!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hr7cwsn62yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ggf2jf</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Press On Nail artists</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggf2jf/press_on_nail_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ggfkri</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Discolored Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggfkri</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ggfzt6</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>2 week old nails peeling. Salon says it's normal .. 1st picture is what I sent to them when the nails were 5 days old, ended up having to file it cause dirt kept getting trapped (last pic)</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggfzt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ggg8ig</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>HOW DO I FIX THIS</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6f8zptbot3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ggde40</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>First time using the stand!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggde40</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1gge1tf</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dip question </t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gge1tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1gggm26</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>new nails 💋</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7jgcafkw3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ggfvai</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat Eye Jack O Lantern Nails I did on myself!  </t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e9ocjibpq3yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ggfjnu</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My version of aura nails </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4ily47bo3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ggf8zt</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60gk81czl3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ggefk3</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>First set on myself</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggefk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ggea0o</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Que les parece?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3oxdjywzd3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ggdcsl</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really liked these pictures I took of my friend’s Halloween nails :) </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggdcsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ggd9c5</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Tried out some new gel as an amateur!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atxtqfyy43yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ggcykz</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I being too picky? </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggcykz</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ggbzzj</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloween everyone! </t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fypbpx8as2yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ggbdvs</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Hand painted looooove</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggbdvs</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ggau86</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>second time doing my gels</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggau86</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ggat8y</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for hg utensils or products for at home manicure </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ggat8y/looking_for_hg_utensils_or_products_for_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1gg9vzn</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>🎃✨Autumnal Tips &amp; Whimsical Stars✨🎃</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8r3x83j12yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1gg9na4</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>One of my favorite options</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owrfigpyx1yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1gg9l28</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>These glamnetic press ons are so cute</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gg9l28</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ggzcm9</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Happy Holoween!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggzb8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ggxljl</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggxljl</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ggxho8</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>How do you function with long nails???!!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggxho8/how_do_you_function_with_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ggwprz</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Frankenstein inspired</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hslw0vsn7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ggwl3f</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Everchanging Colors of Evermore 🌈 </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gca6up3em7yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ggwlku</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>My manicures used to last a day. This is how it looks now on day 6!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pfixtojm7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ggwe6d</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>My yearly Halloween polish</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0soi9hdk7yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ggvk5h</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Another late night Halloween nails post! (tw: fake blood second photo and on)</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggvk5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ggvbi2</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Metallic vs Pearl</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggvbi2/metallic_vs_pearl/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ggvarn</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Getting my Halloween nails in before it hits midnight</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggvarn</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ggv0ye</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Molten Sky 😍</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r61boc6c67yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1gguzvz</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r25l8pj267yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ggux41</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Happy Halloween, some dripping nails to celebrate the day ❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggux41</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ggua1s</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>I was so looking forward to this day. To the person that wrote the note....yes....yes indeed.</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggua1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ggu73z</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>October Mani Round Up</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggu73z</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ggtpkb</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>DVN Customer Service Question</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggtpkb/dvn_customer_service_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ggtjzx</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Happy Halloween everyone!!!</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggtjzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ggtg59</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Skittle </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggtg59</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ggtbh2</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Shadowforged Shorties</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggtbh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ggt3cy</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Cirque Delivery Today</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggt3cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ggsr52</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>October manis</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kplh34vqk6yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ggsmn9</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>a perfect rainy autumn day  🌧🍂🔥</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsmn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ggsk4y</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>LynB Beetlejuice Holo-ween Mystery Box: Complete Set</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsk4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1ggsd5k</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Halloween Hobbies</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsd5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1ggsbm3</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Pleasantly surprised by my BKL Craft freebie, Exorcise your rites</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsbm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1ggs582</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Dupe for Essie’s playing koi?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di36zuvpf6yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1ggrnrr</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggrnrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1ggrgxu</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Vampire style 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggrgxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ggq8h2</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hell is empty and all the devils are here 🔥 </t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggq8h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ggq4hy</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>👻 Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggq4hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ggq3s9</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Happy Halloween everybody!🦇</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69gofspxx5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ggpyx5</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Pulled out the spooky polishes for today</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggpyx5/pulled_out_the_spooky_polishes_for_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ggpxx3</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Dark Academia Halloween</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggpxx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ggpveg</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Cirque Dusky Skies 💜✨</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn3vwkv0w5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ggpslh</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>fav color currently</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9viue6wdv5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ggpnw4</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Looking for a vibrant purple/violet</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggpnw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ggp2n8</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My first Mooncat mani for Halloween 👻</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggp2n8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ggp1yb</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">okay yeah happy halloween i guess (nail break👻) </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lunv3ggp5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ggoq3e</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Spiderweb Nails for Halloween! 🕸🕷</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggoq3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ggoa1e</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Nail polish to match this flower?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g73xajfaj5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ggo9wa</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Halloween Nails 🎃</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggo9wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ggo49p</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Told the northern lights to keep shining</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggo49p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ggo12z</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>glowy tahitian pearl vibes w/ revlon amethyst smoke</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggo12z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ggnqpg</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I have a Swamp Gloss problem</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggnqpg/i_have_a_swamp_gloss_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ggnq77</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>💀Happy Halloween💀</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tf4mkckze5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1ggn8vm</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>The spookiest thing to happen to me all day 😱</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml4m6utfb5yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1ggn5n1</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Halloween kitties!</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggn5n1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1ggmrmx</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>The perfect Halloween color</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggmrmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ggmq07</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Which moon cat polishes would look best in cool olive skin?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggmq07</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ggmlj2</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Topper swatch requests!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggmlj2/topper_swatch_requests/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ggm08w</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Nakey nakey!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty2kq13x15yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1gglwmv</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Metallic Blue 💙</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gglwmv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1gglp66</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Patchwork halloween</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gglp66</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ggloix</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Happy Halloween! 🎃</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqsq1zqcz4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ggll4u</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something something Holo-ween! </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggll4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ggli9x</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>A Magical Polish Fit for a Witch</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggli9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ggl98q</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>I just thrifted these for 2$ a bottle!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tesm9i3w4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ggkz3h</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>How do you clean a reusable sponge?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggkz3h/how_do_you_clean_a_reusable_sponge/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ggkody</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>What is the Best Light to Charge GITD Polish?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggkody/what_is_the_best_light_to_charge_gitd_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ggkj8d</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Best base colour for duo chrome?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggkj8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ggkgfx</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I found a car in the wild that matches my nails!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggkgfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ggkdlo</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Best nail strengtheners: trying to grow out my natural nails.</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggkdlo/best_nail_strengtheners_trying_to_grow_out_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ggkayu</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Video of Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wac7wx5po4yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ggk3mn</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfurhf7bn4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ggjyyj</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Imperfect and last minute Halloween, with glow in the dark!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggjyyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ggjlni</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like it with the flash on </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om2bqoufj4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ggjejd</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Diwali + Halloween: an attempt was made</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/01ho2u6wh4yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1gfs1sz</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>First autumn color 🍁</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfs1sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1gfsciy</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 🎃 </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gfsciy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1ggixer</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Nail Fail! Oh I just CANNOT 🤣</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggixer</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ggiu3i</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone used dazzle dry nail color without the rest of the system? </t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ggiu3i/has_anyone_used_dazzle_dry_nail_color_without_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ggid5n</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Love this color for Halloween! Arcana Lacquer Edict of Bane</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/aIklDmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1gghlk8</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Mooncat Lust for Vengeance🧞‍♀️</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gghlk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ggh6yb</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>My October nails (+ growth tracker of the nails AND the plant.)</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggh6yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1gggsqx</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Happy Halloween, everybody! 🎃👻💀🧛‍♀️🧙🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gggsqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ggg99d</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">And the Shadows Flee Away </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggg99d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ggenzo</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>My Halloween/Samhain nails 🥰🎃🧡🖤</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggenzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ggelzb</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Move over, HoH!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggelzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ggefzv</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Sour Apple Halloween!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggefzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1gge7nq</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>It’s freakin’ bats! I love Halloween 🦇</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gge7nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ggdk3f</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Conflicting advice regarding when to apply quick-dry or no-chip top coats to minimize polish shrinkage. What has been your experience?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6p14j8r73yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ggcda5</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Icky halloween nails hehe &gt;:)</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdfik418w2yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ggbk0n</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Shorty manis in October (or, why are all my Halloween polishes flakies?!)</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggbk0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ggbfvs</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Happy Diwalloween 🎃✨</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h759lgc2m2yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1gg9t34</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Halloween Nails (TW: crackle polish)</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubpotwfd02yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ggvzf5</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For my spooky boi </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggvzf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1gguppq</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Ghost Nails! 👻</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfkh2oba37yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1gguoh0</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>👻👻👻</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5fkc6t6x27yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ggulpz</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>RIP Oogie Boogie... By @kalsrebelliousnails on IG</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggulpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ggsrba</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patchwork shiny pants. </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsrba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ggsa1r</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green and white Christmas Teddy Bear </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggsa1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1ggkuer</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Tortoise and gold! 🐢✨</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngb7zb61t4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ggkmhj</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky glow in the dark nails. Happy Halloween 🎃 </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggkmhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ggk6nw</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Something for Dia de los Muertos</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggk6nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ggjk22</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>ℍ𝕒𝕡𝕡𝕪 ℍ𝕒𝕝𝕝𝕠𝕨𝕖𝕖𝕟</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dffhiem3j4yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ggjbm2</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Halloween bats set</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggjbm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ggihrk</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Last Halloween set.</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vagqugmva4yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1gghdc4</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted to share some of my favorite gelx sets that I've done! All hand painted! </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gghdc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ggg7mb</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Halloweeeeeeeen!!!! </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggg7mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ggfxop</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made by me </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2ao0vacr3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ggfnms</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spirited Away nails for Halloween </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meibpa17p3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ggfk95</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My version of aura nails </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0f7egsfo3yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ggbq02</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Birthday NAILS 👻</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggbq02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ggbnl1</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Animal </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25scnn1lo2yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ggay77</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queen of the damned 2 </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ggay77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ggao4f</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Tried this diy nail art from a regular tape~ plz ignore my uneven nails😭 they chip too often💀</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba1xk0nac2yd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1gga4xa</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Sakura cherry blossom nails </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gga4xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1gga275</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aqua cat eye XXXL Stilettos </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gga275</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov  2 08:10:06 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1088"/>
+  <dimension ref="A1:C1250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18929,6 +18929,2760 @@
         </is>
       </c>
     </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ghqnjw</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is this green? </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghqnjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ghrkku</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Are these mediocre?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np164amv2gyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ghr93n</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Fingers and toes!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiz1owk7yfyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ghr3mq</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butterfly loved my nail colour </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f8rgg91wfyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ghqyuq</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Scream nails</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vbvkhm6ufyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ghqsh5</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tried to do something at home for the first time, how did i do? </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yku4fprsrfyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ghq6ne</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Kiara sky dip base broken bottle</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2sl4ymmjfyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ghprcw</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crab pose </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6ru16w5efyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ghoxyc</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lemons </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghoxyc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ghok09</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Emerald Green. A fav 🍀💚</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykzi9qb40fyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ghno79</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Custom Halloween press ons 🎃🖤</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghno79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ghna72</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Milky nails</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq7dj0lxmeyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ghn5in</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>glitzy neutral natural nails✨️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8r32s4xnleyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ghmwgw</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>My Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vuq76a6jeyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ghmgju</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>in November, we wear purple 💜</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghmgju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ghm5u1</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Birthday Nail Ideas?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghm5u1/birthday_nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ghlte0</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2po6t1uu8eyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ghlt9r</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape best suits me? Been doing my own GelX-style nails for a few months after years of salon acrylics </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghlt9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ghl6y9</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>My latest set - ready for November 🤎</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ftiae5z2eyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1ghkvr3</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>The nails I did today for a friend!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjokkml40eyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ghkbsz</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>I’m obsessed with the bears! 🧸💜</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghkbsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ghij42</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Pls help</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghij42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ghk0fr</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been trading my baked goods in exchange for getting my nails done! </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghk0fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ghjxxh</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make press ons last for weeks? </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghjxxh/how_to_make_press_ons_last_for_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ghjxho</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Yall my nail lady doesn’t do drawings and I wanted designs sometimes but she’s a min walk from my home so it’s easy idk if to change her or not</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghjxho/yall_my_nail_lady_doesnt_do_drawings_and_i_wanted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ghjogq</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Press on nails gone wrong. What now?!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghjogq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ghj6i6</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new nails for november </t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghj6i6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ghirhv</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Autumn nails 🍂🍁</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3has9jnyhdyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ghidob</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Solid Glue for Press-Ons</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghidob/solid_glue_for_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ghi2i3</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Gel x set, what do we think?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxuain58cdyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ghhzte</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>A little summer to my fall manicure 🐢🌺</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oi1vvvdbdyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ghhugx</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Cursed... sort of</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghhugx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ghht32</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO recommendations for neutral nail shades for fair skin with cool undertone </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghht32/iso_recommendations_for_neutral_nail_shades_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1ghfsze</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails cracking/splitting? </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghfsze/nails_crackingsplitting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ghfujh</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HOW DO I PREPARE FOR MY FIRST EVER APPOINTMENT!! </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghfujh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ghgmok</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to show off these nails i did on myself </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8k1unk50dyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ghhezw</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Questions about press-ons</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghhezw/questions_about_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ghhe4s</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>haven’t posted my nails in a while, but i needed to share my newest set 💖</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghhe4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ghh3yw</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm so happy with my nails. </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5u12i9w64dyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ghfvud</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice needed for new nail tech. </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghfvud/advice_needed_for_new_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1ghfh84</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w77dtjy3rcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1ghdp3n</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>My nails after climbing 3 times a week for 3 weeks and the new set I got today. I'm in love with the nails my new nailtech makes for me. First set was an inspo from u/KneemaToad and the second was an inspo from u/Lexyevans</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghdp3n/my_nails_after_climbing_3_times_a_week_for_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1ghew9s</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Gel nails lifting. Help!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghew9s/gel_nails_lifting_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ghew27</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Show me your nail design with stickers</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghew27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1gheko0</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth/strengthen tips </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gheko0/nail_growthstrengthen_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ghe0s7</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>New polish</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usnfl9mmfcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ghdhk7</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Extensions that can be removed at home?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghdhk7/extensions_that_can_be_removed_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1ghdbs5</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>My sister went to get a Russian manicure even after I recently told her they're bad</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghdbs5/my_sister_went_to_get_a_russian_manicure_even/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1ghd8jv</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My last set for Baptism party </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n4l4deh9cyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1ghd6rs</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>press on nail artists based in canada?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghd6rs/press_on_nail_artists_based_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1ghcbfk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sending off spooky season with bats 🦇 </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghcbfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1ghbzd3</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Time to dry regular polish at salon?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ghbzd3/time_to_dry_regular_polish_at_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1ghb82j</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know it’s fall but I’m going to Hawaii lol so here are my siren nails inspired by the ocean 🦪✨ last pic for inspo </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghb82j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1gh9nnz</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Never had nails this short before and it feels really uncomfortable</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16w7shn6ibyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1ghahho</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Christmas nails since November.</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb8d9hyfobyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1gha39a</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>I did my mom's nails 💕</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwy7enkglbyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1gh9fx1</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Referral for Joyee Nails</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gh9fx1/referral_for_joyee_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1gh94id</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I knew these press ons reminded me of something </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p482uhm8ebyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1gh94ab</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Where to get Press-On Acrylics?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gh94ab/where_to_get_presson_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1gh90ra</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>advice needed!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh90ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1gh7yr3</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nail snagged bad, need advice on removal </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh7yr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1gh4gas</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Space/galaxy inspired marble gel nails </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh4gas</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1gh8i2o</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Couldn’t decide on a color so we went neutral</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vahfxtm9byd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1gh84da</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feelin spooky! </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f2uj1vq6byd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1gh7h5k</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Happy Halloween!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh7h5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1gh74vy</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Sparkly french ❤️</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ljncbs4zayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1gh720q</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>My nails for this month🦓✨</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xhnoekhyayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1gh6xck</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No more Halloween nails </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnddghwfxayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1gh6r9b</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Style and length... Thoughts/advice? </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of5b7nh1wayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1gh65vd</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Chrome and magnetic cat eye combo</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoilbw9arayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1gh63l5</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve never gotten my nails done before; what’s the process like? </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gh63l5/ive_never_gotten_my_nails_done_before_whats_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1gh5tfr</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How does everyone put shoes and socks back on after a pedicure? </t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gh5tfr/how_does_everyone_put_shoes_and_socks_back_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1gh5gaq</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Just got these done! I’m obsessed with cat eye nails 💚✨</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzfurt3glayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1gh58ak</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Tortoise shell tips with a fleck of gold</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i005akqkjayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1gh4u3c</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>november 1st. 🍁✨</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh4u3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1gh4spm</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>My contribution to spooky season! 🦇</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh4spm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1gh46zs</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Finally tried out Apres tips. I’m in love with the shape.</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1eq8llcaayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1gh3j95</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Anybody saw this work? 🤯</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DBzwaIrMPI3/?igsh=MWYwN2FpMXk2Y20ycA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1gh3fby</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shape feedback </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvm44r5o2ayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1gh3eg5</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Trying to step it up a bit....</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4azboche2ayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1gh2ez0</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>My nails for this Halloween</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh2ez0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1gh2bte</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Just wanted to share my Halloween nails that literally took me all day to do (but absolutely worth it) 👻</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxrafjt0q9yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1gh26bd</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Husband asking for advice </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zy2s9x74o9yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1gh20wm</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>French coffin nails!!</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3nq5515m9yd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1gh1o8t</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Halloween nails based on my eldritch god OC 👁️🦑</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh1o8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1gh0ke0</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh0ke0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ghotp6</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's up with lechat? </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghotp6/whats_up_with_lechat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1ghntbz</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s beginning to feel a lot like Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghntbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1ghmu37</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Does anyone know where I could find Mooncat "Fake Halo"  in Australia? With the currency conversion and shipping it would cost $60 to order from the website! D: But it's perfect and I NEED it</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhhvc9ddieyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1ghm18m</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Black shimmer?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghm18m/black_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1ghlh2w</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🎉🎉</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghlh2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1ghlgac</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Finding Feathers Lacquer (multi-manis)</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghlgac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1ghlg1e</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>October Mani Roundup</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghlg1e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ghldao</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Molten Sky ♥️💙✨</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghldao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1ghl06n</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Best base coats?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghl06n/best_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ghk6g6</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Wanted to share my ghostly manis! 👻</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghk6g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ghjvn4</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why did my nail lift? </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh1obdg6rdyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ghjsaj</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Gel polish bottles</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghjsaj/gel_polish_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1ghjlqh</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Polished for Days Angel Wings</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghjlqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1ghje2r</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(Late) Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuwmt9n4ndyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1ghises</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Obvious tricks that took me too long to learn</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghises/obvious_tricks_that_took_me_too_long_to_learn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1ghil5i</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Harlow &amp; Co ILNP pre-sale dates?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghil5i/harlow_co_ilnp_presale_dates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1ghi66o</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>ISO recommendations for neutral nail shades for fair skin with cool undertone</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghi66o/iso_recommendations_for_neutral_nail_shades_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1ghhn6y</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Homemade tortoiseshell jelly</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghhn6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1gh6dv8</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>is Sally Hansen Mega Shine Discontinued / alternative top coats</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gh6dv8/is_sally_hansen_mega_shine_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1ghgz7v</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Totally Gourd-geous</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghgz7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1ghgbl2</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Testing new nail designs 🩷</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/390w1zhqxcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1ghg6xh</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>I'm in love!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghg6xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1ghg4en</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>PPU order arrived the same day my partner surprised me with the new Mooncat collection 😍</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lrysjl6wcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1ghg2cx</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Thank shit my 2 new pruglies aren't exact dupes! 🙏</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghg2cx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1ghg04x</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Fools paradise cirque color</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/phaq6mz6vcyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1ghfttx</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>First ever nail art for Halloween</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pj2v3a6vtcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1ghfqp4</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>feeling blue (and rainbow)</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghfqp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1gheku2</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Looking for Chanel Ciel de Nuit dupes</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gheku2/looking_for_chanel_ciel_de_nuit_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1gheb1x</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Marshall’s Haul!!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwsxib6vhcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1ghe034</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is going on with my top coat? </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghe034</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1ghdjk6</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Pets, Pumpkins....and a Spider</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghdjk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1ghd8ox</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>What are the best Black Friday Sales?</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghd8ox/what_are_the_best_black_friday_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ghd7pg</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>My October Manis</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghd7pg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1ghc3r7</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does cold weather cause chipping? </t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghc3r7/does_cold_weather_cause_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1ghbzde</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>✨️🦴Glitter Bones🦴✨️</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghbzde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1ghbtf1</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Mooncat H of H</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghbtf1/mooncat_h_of_h/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ghb825</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tkyikgi2ubyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ghameh</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fireworks for Diwali! </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghameh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1gha0gq</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>a month of manis: october!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gha0gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1gh9yml</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>So long, suckers!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8uu0c8fikbyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1gh9422</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Spooky shorties with over a week of wear!</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh9422</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1gh92u7</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>October Manis</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh92u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1gh8r50</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>had to try the ghost tips for halloween</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh8r50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1gh81j9</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Love almost black colors 🖤</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra22jfx46byd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1gh7irm</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>My first PPU order!</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70ph9lm32byd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1gh76sk</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Similar Polish?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hswhq1zjzayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1gh6jdv</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PPU and ordering. A public service announcement. </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gh6jdv/ppu_and_ordering_a_public_service_announcement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1gh619f</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Proximal nail fold pushed up. </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebrf7ghaqayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1gh5t70</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Revlon Daydreamer at sunset!</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q7ei4leoayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1gh5qjd</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What happened? </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98jyo7vsnayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1gh5maw</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>What happened to Color Club: Results from a deep investigation</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gh5maw/what_happened_to_color_club_results_from_a_deep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1gh4qcz</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>november 1st. 🍁✨</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh4qcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1gh3uju</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh3uju</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1gh3u8m</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Should I file down the sides of my nails ( where it curves a bit) ?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gh3u8m/should_i_file_down_the_sides_of_my_nails_where_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1gh3nlw</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Exploded in my hand while opening for the first time. I'm out of polish remover 😑</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh3nlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1gh1vck</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gh1vck/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1gh0v5x</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Maximum Effort Maxim Tomato.</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q8fpyqs869yd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1ghbq27</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Just in time for Halloween! 🕷️🕸️</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2p9ucfwxbyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1ghq21f</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cool cold weather nails </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghq21f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1ghpzl3</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Several Cool Blue </t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghpzl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1ghpwkw</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My take on a Tino Vo design </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghpwkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1ghnqli</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mismatch nail trend </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmi7lp8ireyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1ghnplz</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>I just found this sub, here's some of my mani pics.. :)</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghnplz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1ghnbd5</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last set i had donde in Argentina. Made by my manicurist Micaelamp_nails. </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghnbd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1ghlonf</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Some y2k nails on my practice hand🥰 ig: @hair.with.drew</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghlonf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1ghijqq</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My Halloween nails :)</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae504uh7gdyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1ghhubq</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Some of My Nail Art Over Time</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghhubq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1ghffje</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumnal BIAB </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1fyg2nqqcyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1ghf3pb</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>My spooky set</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghf3pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1gheyxw</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Pokémon Press Ons I Made For a Friend</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gqcmi61ncyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1ghcrnc</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz99ldhs5cyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1ghbv40</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>How to do this type of nail art?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ba5462byybyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1gh7kvn</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>I got up early to make this set, give me your opinion?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2s3nq0k2byd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1gh5o9y</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Blue &amp; Gold to match my Cleopatra Halloween costume 💙💛🦋🌟 (feedback welcome i am a beginner 😭)</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gh5o9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1gh4ww9</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Happy Halloween 🎃</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ron4apdxgayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1gh42ya</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Practice practice practice</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn1yoo199ayd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Nov  3 08:09:39 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_03.xlsx
+++ b/data/collected_data/2024_11_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1250"/>
+  <dimension ref="A1:C1440"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21683,6 +21683,3236 @@
         </is>
       </c>
     </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1gihwsm</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Judge my first self done gelset with press ons</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnxsn83z6nyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1gicku0</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Sculpting Nail Gel/Glue?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gicku0/sculpting_nail_gelglue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1gif6yz</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Weird question</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gif6yz/weird_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1gifmx2</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>What I asked for VS what I got 😅</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gifmx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1gih3lw</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>simple but I just love it &lt;3</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0e0t58mvmyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1gigts7</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I could take out a werewolf with these, I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gigts7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1gigpx8</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>My natural nails after 4 months</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm3mhwdhqmyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1gigfxg</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>So coquetteee</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80bcqrvwmmyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1gigaok</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>My thumbs are 2 different colors…. I went and got them done today and I just noticed it… is it super noticeable and not cute:((</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gigaok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1gifz1m</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Switching from acrylic to gel-x?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gifz1m/switching_from_acrylic_to_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1giety9</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Melody Susie Fleurwee vs Canni</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1giety9/melody_susie_fleurwee_vs_canni/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1giecgn</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to cut down on time? 3 hr set… </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jtm9w2wylyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1gie0yq</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This color makes me feel pretty bad ass </t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xoki1amvlyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1gid4t8</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Does anyone else do this,</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve7fcukimlyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1gieirq</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Emerald marble with a hint of gold ✨</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gieirq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1gie6in</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cats-Eye obsession 💜 </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gie6in</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1gie5gt</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Fill dayyyy</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88cqkdvvwlyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1gie0bg</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Need help w/ press-ons</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gie0bg/need_help_w_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1gids3g</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>My first time making my own press on nails. I'm a little on the fence, Do they look ok?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nuob0pn2tlyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1gidrnf</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>My first time making my own press on nails. I'm a little on the fence, Do they look ok?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/agv8kmwxslyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1gidlla</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s everyone’s go to nail growth serum?! I have 7 months to grow my nails so I don’t need acrylics for my wedding!! </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gidlla/whats_everyones_go_to_nail_growth_serum_i_have_7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1gidgcd</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set color changing black-milky white and one magnetic polish nail </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyuq80nrplyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1gideh9</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last weeks set; self done </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rngx7xj8plyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1gicxfg</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling proud of my homemade manicure </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctee49mgklyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1gicuxi</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Help: Biogel popped off</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gicuxi/help_biogel_popped_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1gicn7w</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>halloween set :)</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ioqef5vqhlyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1gicmer</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>ALWAYS trust the process</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gicmer</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1gickth</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experiences with press on brands? </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gickth/experiences_with_press_on_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1gic6nn</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did my friend's mom's nails! </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17gfobzcdlyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1gibvt1</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>First time getting a manicure. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gibvt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1gibuhl</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Golden Pumpkins</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gibuhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1gia180</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First gel x</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdu77jtptkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1gibjbe</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Gonna be attempting to do rubber base this weekend</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gibjbe/gonna_be_attempting_to_do_rubber_base_this_weekend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1giazao</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Holiday season calls for matching red mani-pedi</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9pssm4l22lyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1giapzz</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Obsessed 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1giapzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1giahfb</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I think im a french mani girl now!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d53ugkpmxkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1gia8ff</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French tip press ons that I painted red. Haven’t had long nails in so long! </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g9ppbvfvkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1gi7pk4</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>What services do I need to ask for?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi7pk4/what_services_do_i_need_to_ask_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1gi6mcy</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Nail Newbie</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi6mcy/nail_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1gi9b23</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Which shape is better?</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi9b23</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1gi9hlu</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polka dot nails </t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi9hlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1gi9fja</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Wanted to share my Halloween press ons before I take them off!! They glow in the dark 😍</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17vyj3wkokyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1gi9dtt</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some snoopy nails </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ietdxs37okyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1gi8oct</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Nail polish color ? [Vids from unhasinteressantes on Instagram]</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m4tzgl3aikyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1gi8k8n</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>🦕</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2q2logahkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1gi8cuc</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>My newest set. I love them!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sqg6sqjfkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1gi854f</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I think I'm finally getting the hang of acrylic 🙏 Opal Acrylic Fade</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyy6m7zqdkyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1gi7yg1</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>new nails 🌌💙🖤</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tll5yi6ckyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1gi6gkf</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Clean slate</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tomwh9yqzjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1ghz9mn</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New hack to clean under nails </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1recrbodiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1gi5v6g</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something wrong with these nails? </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/275yt3nsujyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1gi6kys</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>It’s fall yall</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wjm37lxq0kyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1gi76dp</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Gel Allergy/sensitivity and tips regarding it</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi76dp/gel_allergysensitivity_and_tips_regarding_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1gi5rmx</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Terrifier inspired nails by me!</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi5rmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1gi51j4</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Finally healed my nails!!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yy84trd4ojyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1gi7jte</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Clawwws 🖤✨</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf9oiieq8kyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1gi7aay</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Nails I got done for Halloween!</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0783xxfj6kyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1gi6ys6</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Little late but these are my Halloween/October nails 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bmhdciuv3kyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1gi6uk6</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Started getting my nails done earlier this year, here's some sets I've had </t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6uk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1gi6nk6</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My latest set, matching with the print on this skirt </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6nk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1gi6ca9</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Halloween nails from last week! I love these </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6ca9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1gi6bn0</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aurora borealis nails! </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6bn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1gi6b32</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Black Chutney 🥀</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk0y3zeiyjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1gi68gb</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>New set day!</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edy5kq5xxjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1gi66mz</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(Mani)festing </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edyfgithxjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1gi60q1</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Topaz Tears is sparking with the Autumn Sun.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi60q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1gi5qug</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New GelX Ombre Stiletto Nails...I'm in love! </t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eso8fenstjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1gi5qq1</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lavender fields </t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwdc46prtjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1gi5ojv</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>My natural nails. No gel, no acrylic, just polish.</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dla86on8tjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1gi5mjb</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall flowers 🌺 </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi5mjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1gi53r6</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Simple &amp; iridescent 🩵✨🪩</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tazhm3hmojyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1gi4w9t</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good builder gel/ base coat to present breakage and promote nail growth? </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi4w9t/good_builder_gel_base_coat_to_present_breakage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1gi4q8j</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Best starter acrylic kit?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi4q8j/best_starter_acrylic_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1gi4po3</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Chrome First Timer</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi4po3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1gi4nlp</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Anybody else competing in NNN?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi4nlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1gi4kg2</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November fall colour </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi4kg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1gi4hk0</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Gel Question</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgfivhqojjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1gi47yo</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was feeling a fall colour ! </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2pi5xjzihjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1gi4668</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Sparkly Nails </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdwaks03hjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1gi3rqn</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>First Halloween set on myself 🎃</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/maa87rutdjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1gi3ntg</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Temporary cover-up???</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi3ntg/temporary_coverup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1gi3eio</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Yesterday's set</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi3eio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1gi1r86</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>ELI5: why can't I reuse press-ons with nail glue?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi1r86/eli5_why_cant_i_reuse_pressons_with_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1gi2sh9</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Brown n Gold Nails</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9tl42p16jyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1gi2ty6</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>What am I doing wrong? My chrome powder keeps sticking to the matte layer underneath :(</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi2ty6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1gi2fuj</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>How to tell which nail shape best suits me?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi2fuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1gi2e4v</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>A tribute to the trees that survived 35 mph winds to still have leaves</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glcjgyau2jyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1gi2422</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Gold accents … 😌</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xe6tiul0jyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1gi22bu</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>It's prettier with the little heart 💕</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qm5ouz380jyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1gi1tkt</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Feeling classy in red💅</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1tkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1gi1szt</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Feeling cozy in these!</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1szt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1gi1rd0</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Question about press ons/full coverage tips</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhe7xo0qxiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1gi1hxo</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>What to do after removing acrylics?</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi1hxo/what_to_do_after_removing_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1gi13m1</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Challenged myself with some My little pony nail art. All hand painted by me! </t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpkxpqbesiyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1gi0vrj</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Did my gfs nails for a rave.</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi0vrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1gi0u0x</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Want to buy a pack of unpainted Press ons…any recommendations?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gi0u0x/want_to_buy_a_pack_of_unpainted_press_onsany/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1gi0tuw</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">simple and shiny transition in to november after halloween nails </t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nrnhps9qiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1gi0rys</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Made my sister’s nails today🌅</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi0rys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1gi0otr</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>🌷</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi0otr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1gi00wl</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>First mani in 3 years! Feels so good</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi00wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1gigftx</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>What i ordered vs what I recived.</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gigftx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1gifo87</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>In love with this Lyn B thermal</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gifo87</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1gifiom</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October manis </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gifiom</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1gifg6m</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First 'Polish Pick Up' order </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5shoym5ramyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1gieql3</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Welcome to the Witching Hour </t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3puehnsy2myd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1gieew7</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>I was going for sea glass...I got cucumber</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gieew7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1gid7pc</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know of any dupes for something like these two colours in Australia? Thank you! </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gid7pc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1gics98</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whatcha Psychedelic </t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnyy0l32jlyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1gicovx</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pls be honest with me - does this polish color look okay or does it make my nails look dirty? Feeling discouraged :( </t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gicovx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1gicanu</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gicanu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1gic1os</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">similar polishes but in purple? </t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqrfsbx0clyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1gibugl</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mani after big chop </t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjl6d2l5alyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1gib6sj</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Morticia Addams reds?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gib6sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1giarlk</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Thick polishes</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1giarlk/thick_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1giard5</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>My fiance has been practicing his film photography and got a great photo of my birthday mani</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y56kpw320lyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1giaea4</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer scam alert! </t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8blk5bvwkyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1gi9e5y</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>My friend said these look like a candle flame 🕯️</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi9e5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1gi93mi</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Pink Diamonds</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi92ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1gi91n5</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>First Bee’s Knees Lacquer order, I have no regrets</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sixragselkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1gi8jda</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Rougenoir</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi8jda</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1gi8d2e</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>😭😭😭two lost in one day</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/606e9z5mfkyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1gi84uv</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chamaeleon - Sunset Bliss </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi84uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1gi829c</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>How long does glow polish last</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi829c/how_long_does_glow_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1gi7u8p</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Set! Just having fun but we all start somewhere! </t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9xbq0uyakyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1gi7s41</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your fave brands and colors for neutral polish for fair skin with cool undertone? </t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi7s41/what_are_your_fave_brands_and_colors_for_neutral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1gi7q8i</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Vortex mixers</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi7q8i/vortex_mixers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1gi7mvs</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for tips and suggestions for my 3 year old niece’s Xmas gift. </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi7mvs/looking_for_tips_and_suggestions_for_my_3_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1gi7k5u</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>ILNP grapevine 🍇 💟</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi7k5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1gi6w4v</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Want to try boutique-indie brand </t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6w4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1gi6pj1</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dam— how do I unread this </t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ch6xohq1kyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1gi6n28</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Real gold flakie topper</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi6n28</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1gi6ihc</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Riddle Me This by ILNP</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/epybzaq20kyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1gi675t</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Advice</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi675t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1gi65ak</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Midnight ✨🌘</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi65ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1gi4v0g</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixed feelings on Birthday Nails </t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi4v0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1gi4m3m</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November fall colour </t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi4m3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1gi45ur</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Leaves don't fall in SoCal but I can pretend</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g3m2wo1hjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1gi3xte</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Elsa vibes ❄️</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5y5x7h7fjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1gi3put</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Polished for the Polls!</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9rc3dxedjyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1gi3izt</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/285sgk8wbjyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1gi3h48</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Shaping nails tip</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi3h48/shaping_nails_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1gi32l1</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>❄️ Icy look for 1st Nov mani</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi32l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1gi2z0v</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Fall Nails</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hce6d25i7jyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1gi2nu0</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Have you ever been in love? </t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opx21pzw4jyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1gi2li9</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Nail polish ALWAYS makes my nails peel?</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi2li9/nail_polish_always_makes_my_nails_peel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1gi1xmy</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Fall Mani</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1xmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1gi1sg5</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">just obsessed with my november nails </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1sg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1gi1fr7</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Love this combo!</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1fr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1gi1d9n</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>My favorite October set 😍✨</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi1d9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1gi18kn</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix Indie PPU, Nichibotsu, Velvetized </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi18kn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1gi0sef</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Holo Taco vs. ILNP</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi0sef/holo_taco_vs_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1gi08ed</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Jojoba transparency</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gi08ed/jojoba_transparency/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1ghzxv8</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Advent calendar drops round up?</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghzxv8/advent_calendar_drops_round_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1ghyn2l</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>ILNP/HT dupes for Goblins and Ghoulies and Fae or Foe</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghyn2l/ilnpht_dupes_for_goblins_and_ghoulies_and_fae_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1ghn3ms</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Halloween spiderweb nail art!</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghn3ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1ghyf3q</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t xml:space="preserve">She’s bubbly but she’s cute </t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddag05pt6iyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1ghygbb</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In honor of me and my partners interests. </t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgsrupj37iyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1ghyeyq</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Watermelon shifty</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghyeyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1ghyeej</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina - Counting My Blessings</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghyeej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1ghyb2x</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Looking for...</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghyb2x/looking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1ghxvmf</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>First November Mani</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pma2kadd2iyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1ghxo45</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>ILNP Pyro ♡</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghxo45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1ghwkwj</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>So happy with this nail art 💜</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghwkwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1ghwjdh</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>ISO: Warm purple multichrome/shimmer/magnetics</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ghwjdh/iso_warm_purple_multichromeshimmermagnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1ghwdii</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>First successful attempt at fluid nail art</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghwdii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1ghvqf3</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghvqf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1ghv872</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>ILNP poison (cateye magnet)</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghv872</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1ghuz1c</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All of my October Manis </t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghuz1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1ghuiy3</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Whatcha + Cat Tax</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghuiy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1ghu2eg</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>What I wore in October</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghu2eg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1gibx89</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Golden Pumpkins</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gibx89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1gib0ip</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Third time using gel polish, even tried out a shell thread gel on the pinky</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bti9xkdd2lyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1gi93rx</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Reputation Inspired Snake Nails</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi93rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1gi7baf</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>November Gel Gold Chrome</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7tn3nbwp6kyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1gi5vps</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adding 2 pictures to the Twisted Tea </t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi5vps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1gi4b4n</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Nais</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrjyi659ijyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1gi3uk5</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Advice / recommendations please :)</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gi3uk5/advice_recommendations_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1gi2pem</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What Am I doing wrong? The chrome powder keeps sticking to the matte layer underneath :( </t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi2pem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1gi1njp</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>SPOOKED NAILS!👻💀🎃</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we5lpqtvwiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1gi0zbo</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>My Halloween 👻 Nails</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gi0zbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1ghywjz</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0plr9akraiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1ghyts4</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mecq8e4aiyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1ghwmmu</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So happy with how these turned out! </t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghwmmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1ghutwh</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>IT inspired nail I did 🤡</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53uhh9a1ahyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1ghv2p0</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Happy (late) halloween! 🤡</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f7gwganchyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1ghvnot</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Elmo + Cookie monster!!! 💙❤️</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ibp3it1oihyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1ghvi73</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Twisted Tea anyone </t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghvi73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1ghvf00</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Land Before Time </t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghvf00</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1ghsb3r</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>Trying to perfect my blobs</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghsb3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1ghs73p</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cursed pose... sort of </t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ghs73p</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>